<commit_message>
Added new Test case files
</commit_message>
<xml_diff>
--- a/final-framework-testng/resources/RetailTestcasesData.xlsx
+++ b/final-framework-testng/resources/RetailTestcasesData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VandanaKapoor\git\ManipalUpskillProject\final-framework-testng\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F12F39C-FAC4-4D6E-A828-F2FA66D8DD79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14759C3-29D2-4C46-A7E3-714AEFAACA62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{3050079E-1AC9-4733-A645-5F7107A7FE03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="3" xr2:uid="{3050079E-1AC9-4733-A645-5F7107A7FE03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="UsersData" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Tester1</t>
   </si>
@@ -44,6 +46,36 @@
   </si>
   <si>
     <t>abc1@test.com</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>Test1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>www.gmail.com</t>
+  </si>
+  <si>
+    <t>Runfast7#123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t>Electronic city</t>
+  </si>
+  <si>
+    <t>immediate</t>
+  </si>
+  <si>
+    <t>yeshwanthapur</t>
+  </si>
+  <si>
+    <t>Test launch1234</t>
   </si>
 </sst>
 </file>
@@ -408,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0F7A48-AA6B-40D1-A5AE-5CBA6885E3ED}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -463,4 +495,100 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0A2F50-2D9E-4246-A900-EE02831791F9}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{908B6F33-C536-4510-962F-DF373D3924F0}"/>
+    <hyperlink ref="E1" r:id="rId2" xr:uid="{9AB7CFC9-10E7-4E44-801B-271295EFD07F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92063B73-3C45-40DE-A825-1ECE6091888A}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1">
+        <v>50000</v>
+      </c>
+      <c r="C1">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>120</v>
+      </c>
+      <c r="J1">
+        <v>56</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the test case files
</commit_message>
<xml_diff>
--- a/final-framework-testng/resources/RetailTestcasesData.xlsx
+++ b/final-framework-testng/resources/RetailTestcasesData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VandanaKapoor\git\ManipalUpskillProject\final-framework-testng\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14759C3-29D2-4C46-A7E3-714AEFAACA62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A112DF-0855-4681-AE7A-C959E80E45C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="3" xr2:uid="{3050079E-1AC9-4733-A645-5F7107A7FE03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="2" xr2:uid="{3050079E-1AC9-4733-A645-5F7107A7FE03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="UsersData" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Tester1</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>Test launch1234</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>selenium@gmail.com</t>
+  </si>
+  <si>
+    <t>apartment</t>
+  </si>
+  <si>
+    <t>looking for apartment</t>
   </si>
 </sst>
 </file>
@@ -501,9 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0A2F50-2D9E-4246-A900-EE02831791F9}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -546,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92063B73-3C45-40DE-A825-1ECE6091888A}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -591,4 +602,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE113B0-8D53-4D0A-84AC-42B47FD5BAC1}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1">
+        <v>40000</v>
+      </c>
+      <c r="F1">
+        <v>2000</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{22922251-FBD8-4ABB-A4F3-EE4745977FEB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting the final code files
</commit_message>
<xml_diff>
--- a/final-framework-testng/resources/RetailTestcasesData.xlsx
+++ b/final-framework-testng/resources/RetailTestcasesData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VandanaKapoor\git\ManipalUpskillProject\final-framework-testng\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CEF639-B3A7-4064-A869-8B176747CCF9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289EDD9-B436-4D60-BF01-223668C12B0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" firstSheet="4" activeTab="7" xr2:uid="{3050079E-1AC9-4733-A645-5F7107A7FE03}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Tester1</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Customer</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>Raj123#Mariya</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +937,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,21 +989,36 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{49C336F7-BB1B-4810-840F-6486EBDCD6C1}"/>
     <hyperlink ref="E1" r:id="rId2" xr:uid="{E6E4ABF9-BA48-485D-8D84-B7D9C9EC0C32}"/>
     <hyperlink ref="B2" r:id="rId3" display="alex@gmail.com" xr:uid="{8DCDC5BE-47BF-45BA-BCB4-DE23400B9493}"/>
-    <hyperlink ref="E2:E3" r:id="rId4" display="www.google.com" xr:uid="{51D5623D-0888-458D-9E15-999FF2B09787}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{51D5623D-0888-458D-9E15-999FF2B09787}"/>
     <hyperlink ref="F2" r:id="rId5" xr:uid="{6630DF46-BFD8-4C5D-8B56-0E4BA0881EFD}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{0A113288-0C1C-46E4-9AE9-CBE37D1E5039}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>